<commit_message>
attempt to fix pTiR
</commit_message>
<xml_diff>
--- a/bootcamp_collection.xlsx
+++ b/bootcamp_collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/Documents/GitHub/iGEM-bootcamp-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7891814-57EE-3F47-91B7-F9751635EC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F85421-FB3D-AB4D-A533-AE4488EBAEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23624,7 +23624,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24163,7 +24163,7 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>7536</v>
+        <v>7535</v>
       </c>
       <c r="B24" t="s">
         <v>4473</v>
@@ -25394,7 +25394,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25716,7 +25716,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>7536</v>
+        <v>7535</v>
       </c>
       <c r="G14" s="36" t="s">
         <v>7550</v>

</xml_diff>

<commit_message>
set devices as final product
</commit_message>
<xml_diff>
--- a/bootcamp_collection.xlsx
+++ b/bootcamp_collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/Documents/GitHub/iGEM-bootcamp-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BF22B9-CD63-7542-BB7D-B3A4FAEC6E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F3FA56-484D-AF45-8245-C5032F2D105D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25388,7 +25388,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25707,7 +25707,7 @@
         <v>7542</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="36" t="s">
         <v>7535</v>

</xml_diff>

<commit_message>
add in fusion sites
</commit_message>
<xml_diff>
--- a/bootcamp_collection.xlsx
+++ b/bootcamp_collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/Documents/GitHub/iGEM-bootcamp-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F3FA56-484D-AF45-8245-C5032F2D105D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D8B5D6-0D5C-674C-A583-826958F9673A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7637" uniqueCount="7549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7667" uniqueCount="7561">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22752,6 +22752,42 @@
   </si>
   <si>
     <t>Bootcamp devices</t>
+  </si>
+  <si>
+    <t>FSB</t>
+  </si>
+  <si>
+    <t>FSC</t>
+  </si>
+  <si>
+    <t>FSD</t>
+  </si>
+  <si>
+    <t>FSA</t>
+  </si>
+  <si>
+    <t>FSE</t>
+  </si>
+  <si>
+    <t>GGAG</t>
+  </si>
+  <si>
+    <t>TACT</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>GCTT</t>
+  </si>
+  <si>
+    <t>CGCT</t>
+  </si>
+  <si>
+    <t>agagaaagaggagaaatactag</t>
+  </si>
+  <si>
+    <t>aaccaggcatcaaataaaacgaaaggctcagtcgaaagactgggcctttcgttttatctgttgtttgtcggtgaacgctctctactagagtcacactggctcaccttcgggtgggcctttctgcgtttata</t>
   </si>
 </sst>
 </file>
@@ -23617,8 +23653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24086,7 +24122,10 @@
       </c>
       <c r="L21" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>7559</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
@@ -24152,7 +24191,10 @@
       </c>
       <c r="L23" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>131</v>
+      </c>
+      <c r="M23" s="36" t="s">
+        <v>7560</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
@@ -24186,8 +24228,19 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D25" s="5"/>
+      <c r="A25" s="36" t="s">
+        <v>7552</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7445</v>
+      </c>
       <c r="G25" s="5"/>
+      <c r="I25" t="s">
+        <v>7419</v>
+      </c>
       <c r="J25" t="b">
         <v>0</v>
       </c>
@@ -24196,10 +24249,25 @@
       </c>
       <c r="L25" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>7554</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A26" s="36" t="s">
+        <v>7549</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7445</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7419</v>
+      </c>
       <c r="J26" t="b">
         <v>0</v>
       </c>
@@ -24208,11 +24276,25 @@
       </c>
       <c r="L26" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="M26" s="36" t="s">
+        <v>7555</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D27" s="5"/>
+      <c r="A27" s="36" t="s">
+        <v>7550</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7445</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7419</v>
+      </c>
       <c r="J27" t="b">
         <v>0</v>
       </c>
@@ -24221,12 +24303,25 @@
       </c>
       <c r="L27" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="M27" s="36" t="s">
+        <v>7556</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="36"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="36" t="s">
+        <v>7551</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7445</v>
+      </c>
+      <c r="I28" t="s">
+        <v>7419</v>
+      </c>
       <c r="J28" t="b">
         <v>0</v>
       </c>
@@ -24235,12 +24330,25 @@
       </c>
       <c r="L28" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="M28" s="36" t="s">
+        <v>7557</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="36"/>
-      <c r="D29" s="5"/>
+      <c r="A29" s="36" t="s">
+        <v>7553</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7445</v>
+      </c>
+      <c r="I29" t="s">
+        <v>7419</v>
+      </c>
       <c r="J29" t="b">
         <v>0</v>
       </c>
@@ -24249,7 +24357,10 @@
       </c>
       <c r="L29" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="M29" s="36" t="s">
+        <v>7558</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
@@ -25387,8 +25498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25716,12 +25827,21 @@
         <v>7546</v>
       </c>
       <c r="H14" s="36" t="s">
+        <v>7549</v>
+      </c>
+      <c r="I14" s="42" t="s">
         <v>7543</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="J14" s="36" t="s">
+        <v>7550</v>
+      </c>
+      <c r="K14" s="36" t="s">
         <v>7544</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="L14" s="36" t="s">
+        <v>7551</v>
+      </c>
+      <c r="M14" s="36" t="s">
         <v>7545</v>
       </c>
     </row>

</xml_diff>